<commit_message>
Adding sprint numbers to product backlog
</commit_message>
<xml_diff>
--- a/Artifacts/Recypy_Deliverable_1_ProductBacklog.xlsx
+++ b/Artifacts/Recypy_Deliverable_1_ProductBacklog.xlsx
@@ -58,6 +58,9 @@
     <t>As a picky eater, I want to save recipes I like for later so I can make them again.</t>
   </si>
   <si>
+    <t>H</t>
+  </si>
+  <si>
     <t>As a vegan, I want to find only recipes that fit my dietary needs so that I can save time.</t>
   </si>
   <si>
@@ -73,7 +76,7 @@
     <t>As a parent to a picky eater, I want creative ways to sneak vegetables into meals so I can make my kid eat healthier.</t>
   </si>
   <si>
-    <t>As an intense competitor, I want to see how my recipes stack up against other similar ones to validate myself as a chef.</t>
+    <t>As an intense competitor, I want to see how my recipes ratings stack up against other similar ones to validate myself as a chef.</t>
   </si>
   <si>
     <t>As somebody who recently lost their grandma, I want to share her recipes with the world to help keep her memory alive.</t>
@@ -104,9 +107,6 @@
   </si>
   <si>
     <t>As a mother or father, I would like to learn how to cook homemade meals for our family so we don’t have to eat out.</t>
-  </si>
-  <si>
-    <t>H</t>
   </si>
   <si>
     <t>As someone who doesn’t have the time to cook everyday, I would like to find recipes that will give me leftovers so I can get more out of one meal.</t>
@@ -249,7 +249,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -259,44 +259,47 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="5" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="5" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="5" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="5" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -515,17 +518,17 @@
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -553,10 +556,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Arial"/>
-            <a:ea typeface="Arial"/>
-            <a:cs typeface="Arial"/>
-            <a:sym typeface="Arial"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -804,12 +807,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1096,7 +1099,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1124,10 +1127,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Arial"/>
-            <a:ea typeface="Arial"/>
-            <a:cs typeface="Arial"/>
-            <a:sym typeface="Arial"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1385,7 +1388,7 @@
   <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="4.85156" style="1" customWidth="1"/>
-    <col min="2" max="2" width="94.125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="94.1719" style="1" customWidth="1"/>
     <col min="3" max="3" width="18.3516" style="1" customWidth="1"/>
     <col min="4" max="4" width="16.5" style="1" customWidth="1"/>
     <col min="5" max="5" width="15.8516" style="1" customWidth="1"/>
@@ -1420,7 +1423,9 @@
       <c r="B2" t="s" s="4">
         <v>6</v>
       </c>
-      <c r="C2" s="5"/>
+      <c r="C2" s="5">
+        <v>3</v>
+      </c>
       <c r="D2" t="s" s="6">
         <v>7</v>
       </c>
@@ -1438,7 +1443,9 @@
       <c r="B3" t="s" s="9">
         <v>9</v>
       </c>
-      <c r="C3" s="10"/>
+      <c r="C3" s="10">
+        <v>5</v>
+      </c>
       <c r="D3" t="s" s="11">
         <v>7</v>
       </c>
@@ -1456,7 +1463,9 @@
       <c r="B4" t="s" s="14">
         <v>10</v>
       </c>
-      <c r="C4" s="15"/>
+      <c r="C4" s="10">
+        <v>3</v>
+      </c>
       <c r="D4" t="s" s="11">
         <v>11</v>
       </c>
@@ -1474,7 +1483,9 @@
       <c r="B5" t="s" s="14">
         <v>12</v>
       </c>
-      <c r="C5" s="15"/>
+      <c r="C5" s="10">
+        <v>6</v>
+      </c>
       <c r="D5" t="s" s="11">
         <v>11</v>
       </c>
@@ -1492,7 +1503,9 @@
       <c r="B6" t="s" s="14">
         <v>13</v>
       </c>
-      <c r="C6" s="15"/>
+      <c r="C6" s="10">
+        <v>4</v>
+      </c>
       <c r="D6" t="s" s="11">
         <v>11</v>
       </c>
@@ -1510,9 +1523,11 @@
       <c r="B7" t="s" s="14">
         <v>14</v>
       </c>
-      <c r="C7" s="15"/>
+      <c r="C7" s="10">
+        <v>4</v>
+      </c>
       <c r="D7" t="s" s="11">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="E7" t="s" s="11">
         <v>8</v>
@@ -1526,9 +1541,11 @@
         <v>7</v>
       </c>
       <c r="B8" t="s" s="14">
-        <v>15</v>
-      </c>
-      <c r="C8" s="15"/>
+        <v>16</v>
+      </c>
+      <c r="C8" s="10">
+        <v>3</v>
+      </c>
       <c r="D8" t="s" s="11">
         <v>11</v>
       </c>
@@ -1544,9 +1561,11 @@
         <v>8</v>
       </c>
       <c r="B9" t="s" s="14">
-        <v>16</v>
-      </c>
-      <c r="C9" s="15"/>
+        <v>17</v>
+      </c>
+      <c r="C9" s="10">
+        <v>3</v>
+      </c>
       <c r="D9" t="s" s="11">
         <v>7</v>
       </c>
@@ -1562,11 +1581,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s" s="14">
-        <v>17</v>
-      </c>
-      <c r="C10" s="10"/>
+        <v>18</v>
+      </c>
+      <c r="C10" s="10">
+        <v>2</v>
+      </c>
       <c r="D10" t="s" s="11">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="E10" t="s" s="11">
         <v>8</v>
@@ -1580,9 +1601,11 @@
         <v>10</v>
       </c>
       <c r="B11" t="s" s="14">
-        <v>18</v>
-      </c>
-      <c r="C11" s="15"/>
+        <v>19</v>
+      </c>
+      <c r="C11" s="10">
+        <v>3</v>
+      </c>
       <c r="D11" t="s" s="11">
         <v>7</v>
       </c>
@@ -1598,9 +1621,11 @@
         <v>11</v>
       </c>
       <c r="B12" t="s" s="14">
-        <v>19</v>
-      </c>
-      <c r="C12" s="15"/>
+        <v>20</v>
+      </c>
+      <c r="C12" s="10">
+        <v>4</v>
+      </c>
       <c r="D12" t="s" s="11">
         <v>11</v>
       </c>
@@ -1616,9 +1641,11 @@
         <v>12</v>
       </c>
       <c r="B13" t="s" s="14">
-        <v>20</v>
-      </c>
-      <c r="C13" s="10"/>
+        <v>21</v>
+      </c>
+      <c r="C13" s="10">
+        <v>5</v>
+      </c>
       <c r="D13" t="s" s="11">
         <v>7</v>
       </c>
@@ -1634,9 +1661,11 @@
         <v>13</v>
       </c>
       <c r="B14" t="s" s="14">
-        <v>21</v>
-      </c>
-      <c r="C14" s="15"/>
+        <v>22</v>
+      </c>
+      <c r="C14" s="10">
+        <v>2</v>
+      </c>
       <c r="D14" t="s" s="11">
         <v>7</v>
       </c>
@@ -1652,9 +1681,11 @@
         <v>14</v>
       </c>
       <c r="B15" t="s" s="14">
-        <v>22</v>
-      </c>
-      <c r="C15" s="15"/>
+        <v>23</v>
+      </c>
+      <c r="C15" s="10">
+        <v>6</v>
+      </c>
       <c r="D15" t="s" s="11">
         <v>7</v>
       </c>
@@ -1670,9 +1701,11 @@
         <v>15</v>
       </c>
       <c r="B16" t="s" s="14">
-        <v>23</v>
-      </c>
-      <c r="C16" s="15"/>
+        <v>24</v>
+      </c>
+      <c r="C16" s="10">
+        <v>7</v>
+      </c>
       <c r="D16" t="s" s="11">
         <v>7</v>
       </c>
@@ -1688,9 +1721,11 @@
         <v>16</v>
       </c>
       <c r="B17" t="s" s="14">
-        <v>24</v>
-      </c>
-      <c r="C17" s="15"/>
+        <v>25</v>
+      </c>
+      <c r="C17" s="10">
+        <v>4</v>
+      </c>
       <c r="D17" t="s" s="11">
         <v>11</v>
       </c>
@@ -1706,9 +1741,11 @@
         <v>17</v>
       </c>
       <c r="B18" t="s" s="14">
-        <v>25</v>
-      </c>
-      <c r="C18" s="15"/>
+        <v>26</v>
+      </c>
+      <c r="C18" s="10">
+        <v>9</v>
+      </c>
       <c r="D18" t="s" s="11">
         <v>11</v>
       </c>
@@ -1724,9 +1761,11 @@
         <v>18</v>
       </c>
       <c r="B19" t="s" s="14">
-        <v>26</v>
-      </c>
-      <c r="C19" s="15"/>
+        <v>27</v>
+      </c>
+      <c r="C19" s="10">
+        <v>9</v>
+      </c>
       <c r="D19" t="s" s="11">
         <v>11</v>
       </c>
@@ -1742,9 +1781,11 @@
         <v>19</v>
       </c>
       <c r="B20" t="s" s="14">
-        <v>27</v>
-      </c>
-      <c r="C20" s="15"/>
+        <v>28</v>
+      </c>
+      <c r="C20" s="10">
+        <v>9</v>
+      </c>
       <c r="D20" t="s" s="11">
         <v>11</v>
       </c>
@@ -1760,9 +1801,11 @@
         <v>20</v>
       </c>
       <c r="B21" t="s" s="14">
-        <v>28</v>
-      </c>
-      <c r="C21" s="15"/>
+        <v>29</v>
+      </c>
+      <c r="C21" s="10">
+        <v>4</v>
+      </c>
       <c r="D21" t="s" s="11">
         <v>11</v>
       </c>
@@ -1778,9 +1821,11 @@
         <v>21</v>
       </c>
       <c r="B22" t="s" s="14">
-        <v>29</v>
-      </c>
-      <c r="C22" s="15"/>
+        <v>30</v>
+      </c>
+      <c r="C22" s="10">
+        <v>9</v>
+      </c>
       <c r="D22" t="s" s="11">
         <v>7</v>
       </c>
@@ -1796,11 +1841,13 @@
         <v>22</v>
       </c>
       <c r="B23" t="s" s="14">
-        <v>30</v>
-      </c>
-      <c r="C23" s="15"/>
+        <v>31</v>
+      </c>
+      <c r="C23" s="10">
+        <v>10</v>
+      </c>
       <c r="D23" t="s" s="11">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="E23" t="s" s="11">
         <v>8</v>
@@ -1816,7 +1863,9 @@
       <c r="B24" t="s" s="14">
         <v>32</v>
       </c>
-      <c r="C24" s="15"/>
+      <c r="C24" s="10">
+        <v>9</v>
+      </c>
       <c r="D24" t="s" s="11">
         <v>11</v>
       </c>
@@ -1834,7 +1883,9 @@
       <c r="B25" t="s" s="14">
         <v>33</v>
       </c>
-      <c r="C25" s="15"/>
+      <c r="C25" s="10">
+        <v>8</v>
+      </c>
       <c r="D25" t="s" s="11">
         <v>7</v>
       </c>
@@ -1852,7 +1903,9 @@
       <c r="B26" t="s" s="14">
         <v>34</v>
       </c>
-      <c r="C26" s="15"/>
+      <c r="C26" s="10">
+        <v>8</v>
+      </c>
       <c r="D26" t="s" s="11">
         <v>11</v>
       </c>
@@ -1870,7 +1923,9 @@
       <c r="B27" t="s" s="14">
         <v>35</v>
       </c>
-      <c r="C27" s="15"/>
+      <c r="C27" s="10">
+        <v>10</v>
+      </c>
       <c r="D27" t="s" s="11">
         <v>11</v>
       </c>
@@ -1888,7 +1943,9 @@
       <c r="B28" t="s" s="14">
         <v>36</v>
       </c>
-      <c r="C28" s="15"/>
+      <c r="C28" s="10">
+        <v>10</v>
+      </c>
       <c r="D28" t="s" s="11">
         <v>11</v>
       </c>
@@ -1906,7 +1963,9 @@
       <c r="B29" t="s" s="14">
         <v>37</v>
       </c>
-      <c r="C29" s="15"/>
+      <c r="C29" s="10">
+        <v>10</v>
+      </c>
       <c r="D29" t="s" s="11">
         <v>7</v>
       </c>
@@ -1924,9 +1983,11 @@
       <c r="B30" t="s" s="14">
         <v>38</v>
       </c>
-      <c r="C30" s="15"/>
+      <c r="C30" s="10">
+        <v>8</v>
+      </c>
       <c r="D30" t="s" s="11">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="E30" t="s" s="11">
         <v>8</v>
@@ -1942,7 +2003,9 @@
       <c r="B31" t="s" s="14">
         <v>39</v>
       </c>
-      <c r="C31" s="15"/>
+      <c r="C31" s="10">
+        <v>6</v>
+      </c>
       <c r="D31" t="s" s="11">
         <v>7</v>
       </c>
@@ -1960,7 +2023,9 @@
       <c r="B32" t="s" s="14">
         <v>40</v>
       </c>
-      <c r="C32" s="15"/>
+      <c r="C32" s="8">
+        <v>7</v>
+      </c>
       <c r="D32" t="s" s="11">
         <v>7</v>
       </c>
@@ -1973,43 +2038,43 @@
     </row>
     <row r="33" ht="17" customHeight="1">
       <c r="A33" s="15"/>
-      <c r="B33" s="10"/>
+      <c r="B33" s="16"/>
       <c r="C33" s="15"/>
       <c r="D33" s="15"/>
       <c r="E33" s="15"/>
-      <c r="F33" s="10"/>
+      <c r="F33" s="16"/>
     </row>
     <row r="34" ht="17" customHeight="1">
       <c r="A34" s="15"/>
-      <c r="B34" s="10"/>
+      <c r="B34" s="16"/>
       <c r="C34" s="15"/>
       <c r="D34" s="15"/>
       <c r="E34" s="15"/>
-      <c r="F34" s="10"/>
+      <c r="F34" s="16"/>
     </row>
     <row r="35" ht="17" customHeight="1">
       <c r="A35" s="15"/>
-      <c r="B35" s="10"/>
+      <c r="B35" s="16"/>
       <c r="C35" s="15"/>
       <c r="D35" s="15"/>
       <c r="E35" s="15"/>
-      <c r="F35" s="10"/>
+      <c r="F35" s="16"/>
     </row>
     <row r="36" ht="17" customHeight="1">
       <c r="A36" s="15"/>
-      <c r="B36" s="10"/>
+      <c r="B36" s="16"/>
       <c r="C36" s="15"/>
       <c r="D36" s="15"/>
       <c r="E36" s="15"/>
-      <c r="F36" s="10"/>
+      <c r="F36" s="16"/>
     </row>
     <row r="37" ht="17" customHeight="1">
       <c r="A37" s="15"/>
-      <c r="B37" s="10"/>
+      <c r="B37" s="16"/>
       <c r="C37" s="15"/>
       <c r="D37" s="15"/>
       <c r="E37" s="15"/>
-      <c r="F37" s="10"/>
+      <c r="F37" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>